<commit_message>
add Sberbank, fix bug with multi displays generation, throw visualization choosing
</commit_message>
<xml_diff>
--- a/tariff_comparer/20190901_Рынок пакеты.xlsx
+++ b/tariff_comparer/20190901_Рынок пакеты.xlsx
@@ -1,25 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED23765E-4CB0-4936-9AA2-FF818B1A604A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="свод" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="280">
   <si>
     <t>Банк</t>
   </si>
@@ -991,11 +997,112 @@
   <si>
     <t>1 200 руб.</t>
   </si>
+  <si>
+    <t>Сбербанк</t>
+  </si>
+  <si>
+    <t>Лёгкий старт</t>
+  </si>
+  <si>
+    <t>Удачный сезон</t>
+  </si>
+  <si>
+    <t>Хорошая выручка</t>
+  </si>
+  <si>
+    <t>Активные расчеты</t>
+  </si>
+  <si>
+    <t>Большие возможности</t>
+  </si>
+  <si>
+    <t>2 мес - 1 руб, с  3 мес - 590 руб.</t>
+  </si>
+  <si>
+    <t>2 мес - 1 руб, с  3 мес - 1090 руб.</t>
+  </si>
+  <si>
+    <t>2 мес - 1 руб, с  3 мес - 2 390 руб.</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>12 990 руб.</t>
+  </si>
+  <si>
+    <t>3% от суммы</t>
+  </si>
+  <si>
+    <t>до 500 тыс. руб. {свыше 500 тыс. руб. в месяц 3% от суммы}</t>
+  </si>
+  <si>
+    <t>250 руб. в месяц / 2 500руб. в год VisaBusiness/MasterCard Business</t>
+  </si>
+  <si>
+    <t>бесплатно Visa Platinum Business / MasterCard Preferred</t>
+  </si>
+  <si>
+    <t>250 руб. в месяц / 2 500руб. в год VisaBusiness/MasterCardBusiness</t>
+  </si>
+  <si>
+    <t>бесплатно Visa Business Momentum / Mastercard Business Momentum</t>
+  </si>
+  <si>
+    <t>3% от суммы, мин. 400 руб.</t>
+  </si>
+  <si>
+    <t>0,5% - до 150 тыс. руб. (для ИП - бесплатно) 1% - от 150 до 300 тыс. руб. 1,7% - от 300 до 1 500 тыс. руб. 3,5% - от 1 500 до 5 000 тыс. руб. 8% - свыше 5 000 тыс. руб.  Через функцию «зарплатный проект» 0,4 % от любой суммы</t>
+  </si>
+  <si>
+    <t>0,5% - до 150 тыс. руб. – для ИП - бесплатно) 1% - от 150 до 300 тыс. руб. 1,7% - от 300 до 1 500 тыс. руб. 3,5% - от 1500 до 5 000тыс. руб. 8% -свыше 5 000тыс. руб. Через функцию «зарплатный проект» 0,4 % от любой суммы</t>
+  </si>
+  <si>
+    <t>0,5% - до 150 тыс. руб. – для ИП - бесплатно) 1% - от 150 до 300 тыс. руб. 1,7% - от 300 до 1 500 тыс. руб. 3,5% - от 1500 до 5 000тыс. руб. 8% -свыше 5000тыс. руб. Через функцию «зарплатный проект» 0,4 % от любой суммы</t>
+  </si>
+  <si>
+    <t>бесплатно - до 300 тыс. руб. 1,7% - от 300 до 1 500 тыс. руб. 3,5% - от 1 500 до 5 000 тыс. руб. 8% - свыше 5 000 тыс. руб. Через функцию «зарплатный проект» 0,4 % от любой суммы</t>
+  </si>
+  <si>
+    <t>БК: 0,15% от суммы Касса: до 100 тыс. руб. включительно: 1% от суммы,
+мин. 150 руб.
+свыше 100 тыс.руб.: 1% от суммы</t>
+  </si>
+  <si>
+    <t>БК: до 50 тыс. руб., {свыше 50 тыс. руб. в месяц 0,3% от суммы} Касса: до 100 тыс. руб. включительно: 0.36% от суммы,
+мин. 150 руб.
+свыше 100 тыс.руб.: 0,3% от суммы</t>
+  </si>
+  <si>
+    <t>БК: до 100 тыс. руб. {свыше 100 тыс. руб. в месяц 0,15% от суммы} Касса: до 100 тыс. руб. включительно: 0.36% от суммы,
+мин. 150 руб.
+свыше 100 тыс.руб.: 0,3% от суммы</t>
+  </si>
+  <si>
+    <t>БК: 0,3% от суммы Касса: до 100 тыс. руб. включительно: 0.36% от суммы,
+мин. 150 руб.
+свыше 100 тыс.руб.: 0,3% от суммы</t>
+  </si>
+  <si>
+    <t>БК: до 500 тыс. руб. {свыше 500 тыс. руб. в месяц 0,3% от суммы} Касса: до 500 тыс. руб. {свыше 500 тыс. руб. в месяц 0,3% от суммы}</t>
+  </si>
+  <si>
+    <t>5% - до 5 млн. руб. 10% - свыше 5 млн. руб.</t>
+  </si>
+  <si>
+    <t>4% - до 2 млн. руб. 5% - от 2до 5 млн. руб. 10% - свыше 5млн. руб.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3% - до 2 млн.руб. 5% - от 2 до 5 млн. руб. 10% - свыше 5млн. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3% - до 2 млн. руб. 5% - от 2 до 5 млн. руб. 10% - свыше 5 млн. </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1134,25 +1241,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1427,21 +1534,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AU13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AZ13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="AS4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F6" sqref="F6:J6"/>
+      <selection pane="bottomRight" activeCell="AV10" sqref="AV10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1492,82 +1599,89 @@
     <col min="47" max="47" width="25.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="30" t="s">
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="26" t="s">
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26" t="s">
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="26" t="s">
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="S1" s="26"/>
-      <c r="T1" s="26"/>
-      <c r="U1" s="27" t="s">
+      <c r="S1" s="27"/>
+      <c r="T1" s="27"/>
+      <c r="U1" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="26" t="s">
+      <c r="V1" s="30"/>
+      <c r="W1" s="30"/>
+      <c r="X1" s="30"/>
+      <c r="Y1" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="Z1" s="26"/>
-      <c r="AA1" s="26"/>
-      <c r="AB1" s="26" t="s">
+      <c r="Z1" s="27"/>
+      <c r="AA1" s="27"/>
+      <c r="AB1" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="AC1" s="26"/>
-      <c r="AD1" s="26"/>
-      <c r="AE1" s="26"/>
-      <c r="AF1" s="26"/>
-      <c r="AG1" s="26"/>
-      <c r="AH1" s="27" t="s">
+      <c r="AC1" s="27"/>
+      <c r="AD1" s="27"/>
+      <c r="AE1" s="27"/>
+      <c r="AF1" s="27"/>
+      <c r="AG1" s="27"/>
+      <c r="AH1" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="AI1" s="27"/>
-      <c r="AJ1" s="27"/>
-      <c r="AK1" s="28" t="s">
+      <c r="AI1" s="30"/>
+      <c r="AJ1" s="30"/>
+      <c r="AK1" s="31" t="s">
         <v>131</v>
       </c>
-      <c r="AL1" s="28"/>
-      <c r="AM1" s="28"/>
-      <c r="AN1" s="26" t="s">
+      <c r="AL1" s="31"/>
+      <c r="AM1" s="31"/>
+      <c r="AN1" s="27" t="s">
         <v>147</v>
       </c>
-      <c r="AO1" s="26"/>
-      <c r="AP1" s="26"/>
-      <c r="AQ1" s="26"/>
-      <c r="AR1" s="26"/>
-      <c r="AS1" s="27" t="s">
+      <c r="AO1" s="27"/>
+      <c r="AP1" s="27"/>
+      <c r="AQ1" s="27"/>
+      <c r="AR1" s="27"/>
+      <c r="AS1" s="30" t="s">
         <v>153</v>
       </c>
-      <c r="AT1" s="27"/>
-      <c r="AU1" s="27"/>
+      <c r="AT1" s="30"/>
+      <c r="AU1" s="30"/>
+      <c r="AV1" s="30" t="s">
+        <v>249</v>
+      </c>
+      <c r="AW1" s="30"/>
+      <c r="AX1" s="30"/>
+      <c r="AY1" s="30"/>
+      <c r="AZ1" s="30"/>
     </row>
-    <row r="2" spans="1:47" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:52" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1709,8 +1823,23 @@
       <c r="AU2" s="14" t="s">
         <v>157</v>
       </c>
+      <c r="AV2" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="AW2" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="AX2" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="AY2" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="AZ2" s="13" t="s">
+        <v>254</v>
+      </c>
     </row>
-    <row r="3" spans="1:47" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:52" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1852,8 +1981,23 @@
       <c r="AU3" s="21" t="s">
         <v>159</v>
       </c>
+      <c r="AV3" s="21" t="s">
+        <v>258</v>
+      </c>
+      <c r="AW3" s="21" t="s">
+        <v>255</v>
+      </c>
+      <c r="AX3" s="21" t="s">
+        <v>256</v>
+      </c>
+      <c r="AY3" s="21" t="s">
+        <v>257</v>
+      </c>
+      <c r="AZ3" s="21" t="s">
+        <v>259</v>
+      </c>
     </row>
-    <row r="4" spans="1:47" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:52" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1928,7 +2072,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="5" spans="1:47" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:52" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -1990,8 +2134,23 @@
       <c r="AS5" s="13"/>
       <c r="AT5" s="13"/>
       <c r="AU5" s="13"/>
+      <c r="AV5" t="s">
+        <v>265</v>
+      </c>
+      <c r="AW5" t="s">
+        <v>262</v>
+      </c>
+      <c r="AX5" t="s">
+        <v>264</v>
+      </c>
+      <c r="AY5" t="s">
+        <v>264</v>
+      </c>
+      <c r="AZ5" t="s">
+        <v>263</v>
+      </c>
     </row>
-    <row r="6" spans="1:47" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:52" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>56</v>
       </c>
@@ -2112,8 +2271,23 @@
       <c r="AU6" s="7" t="s">
         <v>181</v>
       </c>
+      <c r="AV6" t="s">
+        <v>271</v>
+      </c>
+      <c r="AW6" t="s">
+        <v>272</v>
+      </c>
+      <c r="AX6" t="s">
+        <v>273</v>
+      </c>
+      <c r="AY6" t="s">
+        <v>274</v>
+      </c>
+      <c r="AZ6" t="s">
+        <v>275</v>
+      </c>
     </row>
-    <row r="7" spans="1:47" ht="146.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:52" ht="146.25" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -2175,8 +2349,23 @@
       <c r="AS7" s="13"/>
       <c r="AT7" s="13"/>
       <c r="AU7" s="13"/>
+      <c r="AV7" t="s">
+        <v>260</v>
+      </c>
+      <c r="AW7" t="s">
+        <v>266</v>
+      </c>
+      <c r="AX7" t="s">
+        <v>266</v>
+      </c>
+      <c r="AY7" t="s">
+        <v>266</v>
+      </c>
+      <c r="AZ7" t="s">
+        <v>261</v>
+      </c>
     </row>
-    <row r="8" spans="1:47" ht="56.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:52" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -2310,7 +2499,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="9" spans="1:47" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:52" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -2437,8 +2626,23 @@
       <c r="AU9" s="7" t="s">
         <v>176</v>
       </c>
+      <c r="AV9" t="s">
+        <v>267</v>
+      </c>
+      <c r="AW9" t="s">
+        <v>268</v>
+      </c>
+      <c r="AX9" t="s">
+        <v>268</v>
+      </c>
+      <c r="AY9" t="s">
+        <v>269</v>
+      </c>
+      <c r="AZ9" t="s">
+        <v>270</v>
+      </c>
     </row>
-    <row r="10" spans="1:47" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:52" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -2571,9 +2775,24 @@
       <c r="AU10" s="7" t="s">
         <v>178</v>
       </c>
+      <c r="AV10" t="s">
+        <v>276</v>
+      </c>
+      <c r="AW10" t="s">
+        <v>277</v>
+      </c>
+      <c r="AX10" t="s">
+        <v>278</v>
+      </c>
+      <c r="AY10" t="s">
+        <v>278</v>
+      </c>
+      <c r="AZ10" t="s">
+        <v>279</v>
+      </c>
     </row>
-    <row r="11" spans="1:47" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
+    <row r="11" spans="1:52" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
@@ -2608,12 +2827,12 @@
       <c r="T11" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="U11" s="25" t="s">
+      <c r="U11" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="V11" s="25"/>
-      <c r="W11" s="25"/>
-      <c r="X11" s="25"/>
+      <c r="V11" s="29"/>
+      <c r="W11" s="29"/>
+      <c r="X11" s="29"/>
       <c r="AB11" s="7" t="s">
         <v>120</v>
       </c>
@@ -2638,8 +2857,8 @@
       <c r="AT11" s="13"/>
       <c r="AU11" s="13"/>
     </row>
-    <row r="12" spans="1:47" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
+    <row r="12" spans="1:52" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="25"/>
       <c r="B12" s="5"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
@@ -2654,7 +2873,7 @@
       <c r="AT12" s="13"/>
       <c r="AU12" s="13"/>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:52" x14ac:dyDescent="0.25">
       <c r="AN13" s="13"/>
       <c r="AO13" s="13"/>
       <c r="AP13" s="13"/>
@@ -2665,13 +2884,8 @@
       <c r="AU13" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="R1:T1"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="K1:N1"/>
+  <mergeCells count="15">
+    <mergeCell ref="AV1:AZ1"/>
     <mergeCell ref="U11:X11"/>
     <mergeCell ref="Y1:AA1"/>
     <mergeCell ref="U1:X1"/>
@@ -2680,6 +2894,12 @@
     <mergeCell ref="AB1:AG1"/>
     <mergeCell ref="AH1:AJ1"/>
     <mergeCell ref="AK1:AM1"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="O1:Q1"/>
+    <mergeCell ref="R1:T1"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="K1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>